<commit_message>
Update the excel files to reflect the new format
</commit_message>
<xml_diff>
--- a/sample_excel_files/type_1_key.xlsx
+++ b/sample_excel_files/type_1_key.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardopramanasuranta/Documents/Projects-CMUSV/Fall-2020/18980-GRA/pysheetgrader/sample_excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88557EBE-B9CB-3447-89CA-4B25FA952D62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FFE070D-77D7-5D4F-8F2E-AFD5249E1861}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42280" yWindow="10100" windowWidth="21040" windowHeight="12920" xr2:uid="{E0450653-B2D8-E342-9DE9-A7B7C9F37F08}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15600" xr2:uid="{E0450653-B2D8-E342-9DE9-A7B7C9F37F08}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet3_CheckOrder" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,8 +33,66 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Ricardo Pramana Suranta</author>
+  </authors>
+  <commentList>
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{E63694C2-2EEB-3440-B960-B076C27D8E0F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">Rubric:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">	10P-C
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{AEEFB42D-399A-B945-9D3B-DD4A15813FA8}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">Rubric:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">	5P-C
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -54,18 +113,39 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Seq</t>
+  </si>
+  <si>
+    <t>Cell</t>
+  </si>
+  <si>
+    <t>B6</t>
+  </si>
+  <si>
+    <t>Discounted Total</t>
+  </si>
+  <si>
+    <t>B7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -106,6 +186,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -404,16 +488,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3731C799-78A7-C849-8E49-D29CD30B9485}">
-  <dimension ref="A1:B6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3731C799-78A7-C849-8E49-D29CD30B9485}">
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -465,8 +549,57 @@
         <v>19</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <f xml:space="preserve"> 90% * B6</f>
+        <v>17.100000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4541EA95-7D2D-6649-8688-23204E71A725}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update type 1 key from constant to formula-based grading
</commit_message>
<xml_diff>
--- a/sample_excel_files/type_1_key.xlsx
+++ b/sample_excel_files/type_1_key.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardopramanasuranta/Documents/Projects-CMUSV/Fall-2020/18980-GRA/pysheetgrader/sample_excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FFE070D-77D7-5D4F-8F2E-AFD5249E1861}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{029A8366-C447-A049-935D-E5F1D38B2762}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15600" xr2:uid="{E0450653-B2D8-E342-9DE9-A7B7C9F37F08}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="19200" windowHeight="19180" xr2:uid="{E0450653-B2D8-E342-9DE9-A7B7C9F37F08}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -46,7 +46,6 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">Rubric:
 </t>
@@ -56,9 +55,8 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <scheme val="minor"/>
           </rPr>
-          <t xml:space="preserve">	10P-C
+          <t xml:space="preserve">	10P-F
 </t>
         </r>
       </text>
@@ -70,7 +68,6 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">Rubric:
 </t>
@@ -80,9 +77,8 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <scheme val="minor"/>
           </rPr>
-          <t xml:space="preserve">	5P-C
+          <t xml:space="preserve">	5P-F
 </t>
         </r>
       </text>
@@ -146,7 +142,6 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -186,10 +181,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -491,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3731C799-78A7-C849-8E49-D29CD30B9485}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" zoomScale="183" zoomScaleNormal="183" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -569,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4541EA95-7D2D-6649-8688-23204E71A725}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView zoomScale="314" zoomScaleNormal="314" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add SheetGradingOrder sheet to type_1_key.xlsx
</commit_message>
<xml_diff>
--- a/sample_excel_files/type_1_key.xlsx
+++ b/sample_excel_files/type_1_key.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardopramanasuranta/Documents/Projects-CMUSV/Fall-2020/18980-GRA/pysheetgrader/sample_excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{029A8366-C447-A049-935D-E5F1D38B2762}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B50A621-FF97-3D42-8093-CE30D28257C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="19200" windowHeight="19180" xr2:uid="{E0450653-B2D8-E342-9DE9-A7B7C9F37F08}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="15660" xr2:uid="{E0450653-B2D8-E342-9DE9-A7B7C9F37F08}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
-    <sheet name="Sheet3_CheckOrder" sheetId="4" r:id="rId2"/>
+    <sheet name="SheetGradingOrder" sheetId="5" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet3_CheckOrder" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -88,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Name</t>
   </si>
@@ -124,6 +125,12 @@
   </si>
   <si>
     <t>B7</t>
+  </si>
+  <si>
+    <t>Sheetname</t>
+  </si>
+  <si>
+    <t>Sheet3</t>
   </si>
 </sst>
 </file>
@@ -479,10 +486,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B99D51B3-0541-E64C-BE5C-987FFCB28C3F}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3731C799-78A7-C849-8E49-D29CD30B9485}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="183" zoomScaleNormal="183" workbookViewId="0">
+    <sheetView zoomScale="183" zoomScaleNormal="183" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -556,7 +594,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4541EA95-7D2D-6649-8688-23204E71A725}">
   <dimension ref="A1:B3"/>
   <sheetViews>

</xml_diff>

<commit_message>
Update type_1_key.xlsx rubric to use YAML
</commit_message>
<xml_diff>
--- a/sample_excel_files/type_1_key.xlsx
+++ b/sample_excel_files/type_1_key.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardopramanasuranta/Documents/Projects-CMUSV/Fall-2020/18980-GRA/pysheetgrader/sample_excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B50A621-FF97-3D42-8093-CE30D28257C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0FC501D-F1D6-FB4A-8396-7F9CA0184FFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="15660" xr2:uid="{E0450653-B2D8-E342-9DE9-A7B7C9F37F08}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="15820" activeTab="1" xr2:uid="{E0450653-B2D8-E342-9DE9-A7B7C9F37F08}"/>
   </bookViews>
   <sheets>
     <sheet name="SheetGradingOrder" sheetId="5" r:id="rId1"/>
@@ -48,7 +48,7 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t xml:space="preserve">Rubric:
+          <t xml:space="preserve">rubric:
 </t>
         </r>
         <r>
@@ -57,8 +57,25 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t xml:space="preserve">	10P-F
+          <t xml:space="preserve"> score: 10
 </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve"> type: constant
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>unit_tests:</t>
         </r>
       </text>
     </comment>
@@ -70,7 +87,7 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t xml:space="preserve">Rubric:
+          <t xml:space="preserve">rubric:
 </t>
         </r>
         <r>
@@ -79,7 +96,25 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t xml:space="preserve">	5P-F
+          <t xml:space="preserve"> score: 5
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve"> type: formula
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">unit_tests:
 </t>
         </r>
       </text>
@@ -489,7 +524,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B99D51B3-0541-E64C-BE5C-987FFCB28C3F}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -520,8 +555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3731C799-78A7-C849-8E49-D29CD30B9485}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView zoomScale="183" zoomScaleNormal="183" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="183" zoomScaleNormal="183" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>